<commit_message>
cr promenjen na string
</commit_message>
<xml_diff>
--- a/cr-calculator/src/main/resources/templates/ability-modifiers.xlsx
+++ b/cr-calculator/src/main/resources/templates/ability-modifiers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikola\Desktop\cr-calculator\cr-calculator\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFED722-43D5-4096-99AD-1EDB79CCDF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0693C8-73A7-4F2A-973A-11A9073E283A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10275" yWindow="0" windowWidth="16905" windowHeight="15180" xr2:uid="{562F06C8-B895-4767-9533-9D409BFB4F02}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16905" windowHeight="15180" xr2:uid="{562F06C8-B895-4767-9533-9D409BFB4F02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,13 +35,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>minScore</t>
+    <t>modifier</t>
   </si>
   <si>
-    <t>maxScore</t>
+    <t>Min Score</t>
   </si>
   <si>
-    <t>modifier</t>
+    <t>Max Score</t>
   </si>
 </sst>
 </file>
@@ -101,8 +101,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B4D59FE5-1ABC-4158-BF4D-EF71CF775887}" name="Table1" displayName="Table1" ref="B2:D18" totalsRowShown="0">
   <autoFilter ref="B2:D18" xr:uid="{B4D59FE5-1ABC-4158-BF4D-EF71CF775887}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9301566A-DC35-4677-9C6A-D05548D92A01}" name="minScore"/>
-    <tableColumn id="2" xr3:uid="{80587AEC-F1B9-4D41-ACE9-9E8D0F18F5FB}" name="maxScore"/>
+    <tableColumn id="1" xr3:uid="{9301566A-DC35-4677-9C6A-D05548D92A01}" name="Min Score"/>
+    <tableColumn id="2" xr3:uid="{80587AEC-F1B9-4D41-ACE9-9E8D0F18F5FB}" name="Max Score"/>
     <tableColumn id="3" xr3:uid="{E77E1798-DDEE-4A4A-B443-5C541EE97FA9}" name="modifier"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -409,7 +409,7 @@
   <dimension ref="B2:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,13 +419,13 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>